<commit_message>
att 304 e 269
</commit_message>
<xml_diff>
--- a/xerifes.xlsx
+++ b/xerifes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180"/>
+    <workbookView windowWidth="19635" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="511">
   <si>
     <t>Nº</t>
   </si>
@@ -1409,7 +1409,7 @@
     <t xml:space="preserve"> Rachel Ross ..</t>
   </si>
   <si>
-    <t>-Nessa-</t>
+    <t>-I- -DENNISS- -I-</t>
   </si>
   <si>
     <t>Pegasus</t>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>G u i 4 i 2 1</t>
+  </si>
+  <si>
+    <t>- D4C -</t>
   </si>
 </sst>
 </file>
@@ -2722,10 +2725,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E304"/>
+  <dimension ref="A1:E305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" topLeftCell="B144" workbookViewId="0">
-      <selection activeCell="D144" sqref="D144"/>
+    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="C275" sqref="C275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
@@ -7478,6 +7481,20 @@
         <v>495</v>
       </c>
     </row>
+    <row r="305" spans="1:5">
+      <c r="A305">
+        <v>304</v>
+      </c>
+      <c r="B305" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="C305" s="1">
+        <v>45458</v>
+      </c>
+      <c r="E305" t="s">
+        <v>464</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>